<commit_message>
EPBDS-6639 update test to test issue with classloder for multimodule
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-maven-plugin\it\openl-verify-negative\openl-deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-maven-plugin\it\openl-verify-provided-dependency\openl-deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C87C7DD-38A6-4EE3-B51A-0A7F1779CF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D239B32-9516-4205-8782-9FA481188171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Environment</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>= new Foo ($Step1)</t>
+  </si>
+  <si>
+    <t>dependency</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>= doSomething ($Step2)</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -130,6 +142,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,14 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C11"/>
+  <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -429,55 +451,71 @@
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-13474 Return cxf dependency to deployment module in test
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-maven-plugin\it\openl-verify-provided-dependency\openl-deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkalynovskyi/Desktop/work/PROJECTS/OpenL/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D239B32-9516-4205-8782-9FA481188171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262D924C-32AC-7C46-9E93-1EC1F51D9915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="-22620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Environment</t>
   </si>
@@ -67,16 +67,28 @@
   </si>
   <si>
     <t>= doSomething ($Step2)</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>= OpenLUtils.dateToString(new Date(0,0,0))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,27 +146,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,48 +444,48 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -484,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -492,7 +501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -500,7 +509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -508,15 +517,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-13474 Add comments to test, minor fixes
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkalynovskyi/Desktop/work/PROJECTS/OpenL/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262D924C-32AC-7C46-9E93-1EC1F51D9915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A24E4-5932-0845-8406-AAE38F83FBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="-22620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="7580" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>Step4</t>
   </si>
   <si>
-    <t>= OpenLUtils.dateToString(new Date(0,0,0))</t>
+    <t>= OpenLUtils.dateToString(new Date(0))</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
EPBDS-13474 Fix duplicating of the dependencies in the Maven plugin classloader (#830)
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-maven-plugin\it\openl-verify-provided-dependency\openl-deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkalynovskyi/Desktop/work/PROJECTS/OpenL/Util/openl-maven-plugin/it/openl-verify-provided-dependency/openl-deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D239B32-9516-4205-8782-9FA481188171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A24E4-5932-0845-8406-AAE38F83FBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="7580" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Environment</t>
   </si>
@@ -67,16 +67,28 @@
   </si>
   <si>
     <t>= doSomething ($Step2)</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>= OpenLUtils.dateToString(new Date(0))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,27 +146,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,48 +444,48 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -484,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -492,7 +501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -500,7 +509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -508,15 +517,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>